<commit_message>
working on address extensions
</commit_message>
<xml_diff>
--- a/output/NhiPatient.xlsx
+++ b/output/NhiPatient.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="395">
   <si>
     <t>Path</t>
   </si>
@@ -430,19 +430,16 @@
     <t>NHI</t>
   </si>
   <si>
-    <t>The National Health Idenitifier</t>
-  </si>
-  <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="{&amp;quot;system&amp;quot;:&amp;quot;https://standards.digital.health.nz/id/nhi&amp;quot;}"/&gt;</t>
-  </si>
-  <si>
-    <t>identifier</t>
-  </si>
-  <si>
-    <t>Other identifiers that may be exchanged</t>
-  </si>
-  <si>
-    <t>includes dormant and unrelated. Could use identifier.type to distinguish (though an extension might be better as type means something slightly different)</t>
+    <t>The National Health Identifier. This is the 'live' identifier. Any previous merged identifiers will be present in the 'dormant' NHI list.</t>
+  </si>
+  <si>
+    <t>DormantNHI</t>
+  </si>
+  <si>
+    <t>NHIs that were merged with this one</t>
+  </si>
+  <si>
+    <t>Other identifiers that may be exchanged. In this implementation this will only be dormant (or merged) NHI's, and will have a non-empty 'period.end' property.</t>
   </si>
   <si>
     <t>Patient.active</t>
@@ -480,6 +477,9 @@
     <t>Patient.name</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
     <t xml:space="preserve">HumanName {[]} {[]}
 </t>
   </si>
@@ -496,9 +496,6 @@
     <t>Need to be able to track the patient by multiple names. Examples are your official name and a partner name.</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>.patient.name</t>
   </si>
   <si>
@@ -536,6 +533,9 @@
     <t>Patient.gender</t>
   </si>
   <si>
+    <t>gender</t>
+  </si>
+  <si>
     <t>male | female | other | unknown</t>
   </si>
   <si>
@@ -674,7 +674,10 @@
     <t>Patient.address</t>
   </si>
   <si>
-    <t xml:space="preserve">Address {[]} {[]}
+    <t>address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address {[CanonicalType[http://hl7.org.nz/fhir/StructureDefinition/nhiAddress]]} {[]}
 </t>
   </si>
   <si>
@@ -799,7 +802,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-pat-1:SHALL at least contain a contact's details or a reference to an organization {name.exists() or telecom.exists() or address.exists() or organization.exists()}</t>
+pat-1:SHALL at least contain a contact's details or a reference to an organization {name.exists() or telecom.exists() or address.exists() or organization.exists()}ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}</t>
   </si>
   <si>
     <t>player[classCode=PSN|ANM and determinerCode=INSTANCE]/scopedRole[classCode=CON]</t>
@@ -890,6 +893,10 @@
     <t>Patient.contact.address</t>
   </si>
   <si>
+    <t xml:space="preserve">Address {[]} {[]}
+</t>
+  </si>
+  <si>
     <t>Address for the contact person</t>
   </si>
   <si>
@@ -971,8 +978,8 @@
     <t>Many clinical systems are extended to care for animal patients as well as human.</t>
   </si>
   <si>
-    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-</t>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
+ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}</t>
   </si>
   <si>
     <t>player[classCode=ANM]</t>
@@ -1406,7 +1413,7 @@
     <col min="1" max="1" width="38.203125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.8828125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="9.390625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="12.0703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
@@ -2483,10 +2490,10 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>44</v>
@@ -3085,7 +3092,7 @@
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" t="s" s="2">
-        <v>131</v>
+        <v>44</v>
       </c>
       <c r="R15" t="s" s="2">
         <v>44</v>
@@ -3162,13 +3169,13 @@
         <v>120</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C16" t="s" s="2">
         <v>44</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E16" t="s" s="2">
         <v>42</v>
@@ -3189,14 +3196,12 @@
         <v>121</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="L16" t="s" s="2">
         <v>133</v>
       </c>
-      <c r="M16" t="s" s="2">
-        <v>134</v>
-      </c>
+      <c r="M16" s="2"/>
       <c r="N16" t="s" s="2">
         <v>124</v>
       </c>
@@ -3279,7 +3284,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3290,7 +3295,7 @@
         <v>42</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>44</v>
@@ -3302,22 +3307,22 @@
         <v>53</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>136</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>137</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>138</v>
       </c>
-      <c r="M17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>139</v>
       </c>
-      <c r="N17" t="s" s="2">
+      <c r="O17" t="s" s="2">
         <v>140</v>
-      </c>
-      <c r="O17" t="s" s="2">
-        <v>141</v>
       </c>
       <c r="P17" s="2"/>
       <c r="Q17" t="s" s="2">
@@ -3363,7 +3368,7 @@
         <v>44</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>42</v>
@@ -3378,13 +3383,13 @@
         <v>44</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="AK17" t="s" s="2">
+      <c r="AL17" t="s" s="2">
         <v>143</v>
-      </c>
-      <c r="AL17" t="s" s="2">
-        <v>144</v>
       </c>
       <c r="AM17" t="s" s="2">
         <v>44</v>
@@ -3395,15 +3400,17 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" t="s" s="2">
+        <v>145</v>
+      </c>
       <c r="E18" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s" s="2">
         <v>43</v>
@@ -3479,7 +3486,7 @@
         <v>44</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>42</v>
@@ -3494,16 +3501,16 @@
         <v>44</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="AK18" t="s" s="2">
         <v>151</v>
       </c>
-      <c r="AK18" t="s" s="2">
+      <c r="AL18" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM18" t="s" s="2">
         <v>152</v>
-      </c>
-      <c r="AL18" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM18" t="s" s="2">
-        <v>153</v>
       </c>
       <c r="AN18" t="s" s="2">
         <v>44</v>
@@ -3511,7 +3518,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3534,19 +3541,19 @@
         <v>53</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>155</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="L19" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>157</v>
       </c>
-      <c r="M19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>158</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>159</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>44</v>
@@ -3595,7 +3602,7 @@
         <v>44</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>42</v>
@@ -3610,16 +3617,16 @@
         <v>44</v>
       </c>
       <c r="AJ19" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AK19" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="AK19" t="s" s="2">
+      <c r="AL19" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM19" t="s" s="2">
         <v>161</v>
-      </c>
-      <c r="AL19" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM19" t="s" s="2">
-        <v>162</v>
       </c>
       <c r="AN19" t="s" s="2">
         <v>44</v>
@@ -3627,15 +3634,17 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" t="s" s="2">
+        <v>163</v>
+      </c>
       <c r="E20" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F20" t="s" s="2">
         <v>52</v>
@@ -3711,7 +3720,7 @@
         <v>44</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>42</v>
@@ -4093,7 +4102,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s" s="2">
         <v>52</v>
@@ -4320,7 +4329,7 @@
         <v>42</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>44</v>
@@ -4411,7 +4420,7 @@
         <v>205</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>44</v>
@@ -4431,9 +4440,11 @@
       <c r="C27" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" t="s" s="2">
+        <v>208</v>
+      </c>
       <c r="E27" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F27" t="s" s="2">
         <v>43</v>
@@ -4448,19 +4459,19 @@
         <v>53</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>44</v>
@@ -4524,16 +4535,16 @@
         <v>44</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>44</v>
@@ -4541,7 +4552,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4552,7 +4563,7 @@
         <v>42</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>44</v>
@@ -4564,17 +4575,17 @@
         <v>44</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>44</v>
@@ -4602,10 +4613,10 @@
         <v>75</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>44</v>
@@ -4623,7 +4634,7 @@
         <v>44</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>42</v>
@@ -4638,16 +4649,16 @@
         <v>44</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>44</v>
@@ -4655,7 +4666,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4678,19 +4689,19 @@
         <v>44</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>44</v>
@@ -4739,7 +4750,7 @@
         <v>44</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>42</v>
@@ -4754,16 +4765,16 @@
         <v>44</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>44</v>
@@ -4771,7 +4782,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4782,7 +4793,7 @@
         <v>42</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>44</v>
@@ -4794,17 +4805,17 @@
         <v>44</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>44</v>
@@ -4853,7 +4864,7 @@
         <v>44</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>42</v>
@@ -4868,16 +4879,16 @@
         <v>44</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>44</v>
@@ -4885,7 +4896,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4896,7 +4907,7 @@
         <v>42</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>44</v>
@@ -4908,19 +4919,19 @@
         <v>44</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>44</v>
@@ -4969,7 +4980,7 @@
         <v>44</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>42</v>
@@ -4981,13 +4992,13 @@
         <v>44</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>44</v>
@@ -5001,7 +5012,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5012,7 +5023,7 @@
         <v>42</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>44</v>
@@ -5030,7 +5041,7 @@
         <v>187</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5096,7 +5107,7 @@
         <v>44</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>44</v>
@@ -5113,7 +5124,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5139,10 +5150,10 @@
         <v>97</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>118</v>
@@ -5210,7 +5221,7 @@
         <v>44</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>44</v>
@@ -5227,11 +5238,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5256,7 +5267,7 @@
         <v>116</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>118</v>
@@ -5309,7 +5320,7 @@
         <v>44</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>42</v>
@@ -5341,7 +5352,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5352,7 +5363,7 @@
         <v>42</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>44</v>
@@ -5364,17 +5375,17 @@
         <v>44</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>44</v>
@@ -5402,10 +5413,10 @@
         <v>75</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>44</v>
@@ -5423,7 +5434,7 @@
         <v>44</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>42</v>
@@ -5438,16 +5449,16 @@
         <v>44</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>44</v>
@@ -5455,7 +5466,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5466,7 +5477,7 @@
         <v>42</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>44</v>
@@ -5481,14 +5492,14 @@
         <v>146</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>44</v>
@@ -5537,7 +5548,7 @@
         <v>44</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>42</v>
@@ -5552,16 +5563,16 @@
         <v>44</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>44</v>
@@ -5569,7 +5580,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5580,7 +5591,7 @@
         <v>42</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>44</v>
@@ -5592,19 +5603,19 @@
         <v>44</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>44</v>
@@ -5653,7 +5664,7 @@
         <v>44</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>42</v>
@@ -5668,16 +5679,16 @@
         <v>44</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>44</v>
@@ -5685,7 +5696,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5696,7 +5707,7 @@
         <v>42</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>44</v>
@@ -5708,17 +5719,17 @@
         <v>44</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>208</v>
+        <v>278</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>44</v>
@@ -5767,7 +5778,7 @@
         <v>44</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>42</v>
@@ -5782,16 +5793,16 @@
         <v>44</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>44</v>
@@ -5799,7 +5810,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5810,7 +5821,7 @@
         <v>42</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>44</v>
@@ -5828,11 +5839,11 @@
         <v>164</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>44</v>
@@ -5881,7 +5892,7 @@
         <v>44</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>42</v>
@@ -5899,13 +5910,13 @@
         <v>171</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>44</v>
@@ -5913,7 +5924,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5924,7 +5935,7 @@
         <v>42</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>44</v>
@@ -5936,17 +5947,17 @@
         <v>44</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>44</v>
@@ -5995,7 +6006,7 @@
         <v>44</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>42</v>
@@ -6004,22 +6015,22 @@
         <v>52</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>44</v>
@@ -6027,7 +6038,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6038,7 +6049,7 @@
         <v>42</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>44</v>
@@ -6050,13 +6061,13 @@
         <v>44</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -6107,7 +6118,7 @@
         <v>44</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>42</v>
@@ -6122,10 +6133,10 @@
         <v>44</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>44</v>
@@ -6139,7 +6150,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6150,7 +6161,7 @@
         <v>42</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>44</v>
@@ -6162,19 +6173,19 @@
         <v>53</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>44</v>
@@ -6223,7 +6234,7 @@
         <v>44</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>42</v>
@@ -6235,13 +6246,13 @@
         <v>44</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>44</v>
@@ -6255,7 +6266,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6266,7 +6277,7 @@
         <v>42</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>44</v>
@@ -6284,7 +6295,7 @@
         <v>187</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6350,7 +6361,7 @@
         <v>44</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>44</v>
@@ -6367,7 +6378,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6393,10 +6404,10 @@
         <v>97</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M44" t="s" s="2">
         <v>118</v>
@@ -6464,7 +6475,7 @@
         <v>44</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>44</v>
@@ -6481,11 +6492,11 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
@@ -6510,7 +6521,7 @@
         <v>116</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>118</v>
@@ -6563,7 +6574,7 @@
         <v>44</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>42</v>
@@ -6595,7 +6606,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6603,10 +6614,10 @@
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>44</v>
@@ -6618,19 +6629,19 @@
         <v>53</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="O46" t="s" s="2">
         <v>44</v>
@@ -6655,13 +6666,13 @@
         <v>44</v>
       </c>
       <c r="W46" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>44</v>
@@ -6679,7 +6690,7 @@
         <v>44</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>52</v>
@@ -6694,16 +6705,16 @@
         <v>44</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>44</v>
@@ -6711,7 +6722,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6722,7 +6733,7 @@
         <v>42</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>44</v>
@@ -6734,19 +6745,19 @@
         <v>53</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>44</v>
@@ -6771,13 +6782,13 @@
         <v>44</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>44</v>
@@ -6795,7 +6806,7 @@
         <v>44</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>42</v>
@@ -6810,16 +6821,16 @@
         <v>44</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>44</v>
@@ -6827,7 +6838,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6838,7 +6849,7 @@
         <v>42</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>44</v>
@@ -6850,17 +6861,17 @@
         <v>53</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>44</v>
@@ -6885,13 +6896,13 @@
         <v>44</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>44</v>
@@ -6909,7 +6920,7 @@
         <v>44</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>42</v>
@@ -6924,10 +6935,10 @@
         <v>44</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>44</v>
@@ -6941,7 +6952,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6952,7 +6963,7 @@
         <v>42</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>44</v>
@@ -6964,19 +6975,19 @@
         <v>44</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>44</v>
@@ -7025,7 +7036,7 @@
         <v>44</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>42</v>
@@ -7037,13 +7048,13 @@
         <v>44</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>44</v>
@@ -7057,7 +7068,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7068,7 +7079,7 @@
         <v>42</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>44</v>
@@ -7086,7 +7097,7 @@
         <v>187</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -7152,7 +7163,7 @@
         <v>44</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>44</v>
@@ -7169,7 +7180,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7195,10 +7206,10 @@
         <v>97</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M51" t="s" s="2">
         <v>118</v>
@@ -7266,7 +7277,7 @@
         <v>44</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>44</v>
@@ -7283,11 +7294,11 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7312,7 +7323,7 @@
         <v>116</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M52" t="s" s="2">
         <v>118</v>
@@ -7365,7 +7376,7 @@
         <v>44</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>42</v>
@@ -7397,7 +7408,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7405,10 +7416,10 @@
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>44</v>
@@ -7420,19 +7431,19 @@
         <v>44</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>44</v>
@@ -7481,7 +7492,7 @@
         <v>44</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>52</v>
@@ -7496,16 +7507,16 @@
         <v>44</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>44</v>
@@ -7513,7 +7524,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7524,7 +7535,7 @@
         <v>42</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G54" t="s" s="2">
         <v>44</v>
@@ -7536,19 +7547,19 @@
         <v>44</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>44</v>
@@ -7597,7 +7608,7 @@
         <v>44</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>42</v>
@@ -7612,16 +7623,16 @@
         <v>44</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>44</v>
@@ -7629,11 +7640,11 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7652,16 +7663,16 @@
         <v>44</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
@@ -7711,7 +7722,7 @@
         <v>44</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>42</v>
@@ -7726,16 +7737,16 @@
         <v>44</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>44</v>
@@ -7743,7 +7754,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7754,7 +7765,7 @@
         <v>42</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>44</v>
@@ -7766,19 +7777,19 @@
         <v>53</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>44</v>
@@ -7827,7 +7838,7 @@
         <v>44</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>42</v>
@@ -7842,10 +7853,10 @@
         <v>44</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>44</v>
@@ -7859,7 +7870,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7870,7 +7881,7 @@
         <v>42</v>
       </c>
       <c r="F57" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G57" t="s" s="2">
         <v>44</v>
@@ -7882,19 +7893,19 @@
         <v>53</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>44</v>
@@ -7943,7 +7954,7 @@
         <v>44</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>42</v>
@@ -7955,13 +7966,13 @@
         <v>44</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>44</v>
@@ -7975,7 +7986,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7986,7 +7997,7 @@
         <v>42</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G58" t="s" s="2">
         <v>44</v>
@@ -8004,7 +8015,7 @@
         <v>187</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -8070,7 +8081,7 @@
         <v>44</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK58" t="s" s="2">
         <v>44</v>
@@ -8087,7 +8098,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8113,10 +8124,10 @@
         <v>97</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M59" t="s" s="2">
         <v>118</v>
@@ -8184,7 +8195,7 @@
         <v>44</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>44</v>
@@ -8201,11 +8212,11 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -8230,7 +8241,7 @@
         <v>116</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M60" t="s" s="2">
         <v>118</v>
@@ -8283,7 +8294,7 @@
         <v>44</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>42</v>
@@ -8315,7 +8326,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8323,10 +8334,10 @@
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>44</v>
@@ -8338,16 +8349,16 @@
         <v>53</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
@@ -8397,7 +8408,7 @@
         <v>44</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>52</v>
@@ -8415,13 +8426,13 @@
         <v>126</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>44</v>
@@ -8429,7 +8440,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8437,10 +8448,10 @@
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>44</v>
@@ -8455,10 +8466,10 @@
         <v>71</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -8488,28 +8499,28 @@
         <v>168</v>
       </c>
       <c r="X62" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE62" t="s" s="2">
         <v>390</v>
-      </c>
-      <c r="Y62" t="s" s="2">
-        <v>391</v>
-      </c>
-      <c r="Z62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE62" t="s" s="2">
-        <v>388</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>52</v>
@@ -8524,10 +8535,10 @@
         <v>44</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>44</v>

</xml_diff>